<commit_message>
Se han las pruebas de aceptación del sprint 1
Se subieron las pruebas de aceptacion del sprint 1
</commit_message>
<xml_diff>
--- a/Documentos/Pruebas de aceptacion Sprint 1.xlsx
+++ b/Documentos/Pruebas de aceptacion Sprint 1.xlsx
@@ -3,14 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482B4E7A-54A9-4C54-9C6E-E09117F4D564}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E15831-6E86-4058-9126-233A6E2CBB31}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla en blanco" sheetId="1" r:id="rId1"/>
     <sheet name="Publicar Objeto" sheetId="2" r:id="rId2"/>
     <sheet name="Borrar Objeto" sheetId="3" r:id="rId3"/>
+    <sheet name="Editar Objeto" sheetId="4" r:id="rId4"/>
+    <sheet name="Buscar Objeto" sheetId="6" r:id="rId5"/>
+    <sheet name="Buscar por categoria" sheetId="7" r:id="rId6"/>
+    <sheet name="Ver informacion del objeto" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179021" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="119">
   <si>
     <t>PRUEBAS DE ACEPTACION:</t>
   </si>
@@ -170,6 +174,15 @@
     <t>1.7</t>
   </si>
   <si>
+    <t>1.8</t>
+  </si>
+  <si>
+    <t>1.9</t>
+  </si>
+  <si>
+    <t>1.10</t>
+  </si>
+  <si>
     <t>Borrado exitoso</t>
   </si>
   <si>
@@ -191,10 +204,190 @@
     <t xml:space="preserve">EVALUACION: Los objetos que fueron eliminados no volvieron a aparecer en el mercado y tampoco quedo rastro en la base de datos </t>
   </si>
   <si>
-    <t xml:space="preserve">CONDICIONES DE EJECUCION: </t>
-  </si>
-  <si>
     <t>DESCRIPCION: Al presionar el boton de eliminar objeto debe aparecer un cuadro preguntado si se desea realizar la eliminacion, y el usuario debe presionar el boton confirmar para que el objeto se elimine</t>
+  </si>
+  <si>
+    <t>ENTRADAS: Presionar el boton de cancelar objeto  y confirmar la eliminacion.</t>
+  </si>
+  <si>
+    <t>RESULTADO ESPERADO: Aparece el mensaje para confirmar o cancelar la eliminacion del objeto</t>
+  </si>
+  <si>
+    <t>CONDICIONES DE EJECUCION:  Presionar el boton borrar</t>
+  </si>
+  <si>
+    <t>EVALUACION: Al presionar el boton borrar aparece el cuado de texto preguntando si se confirma o no el borrado.</t>
+  </si>
+  <si>
+    <t>Editar objeto</t>
+  </si>
+  <si>
+    <t>Cancelar edicion de objeto</t>
+  </si>
+  <si>
+    <t>DESCRIPCION: El usuario podra editar la informacion de algunos de los objetos que haya publicado con anterioridad.</t>
+  </si>
+  <si>
+    <t>ENTRADAS: Ingresar a la publicacion del objeto a la cual se desea editar su informacion</t>
+  </si>
+  <si>
+    <t>CONDICIONES DE EJECUCION: Ingresar al objeto que se desea Editar su informacion</t>
+  </si>
+  <si>
+    <t>RESULTADO ESPERADO: Que la informacion del objeto sea editada exitosamente</t>
+  </si>
+  <si>
+    <t>EVALUACION: La informacion del objeto publicado es editada correctamente</t>
+  </si>
+  <si>
+    <t>DESCRIPCION: Si el usuario se arrepiente puede cancelar que la publicacion quede guardada con la nueva informacion.</t>
+  </si>
+  <si>
+    <t>CONDICIONES DE EJECUCION: Presionar el boton de cancelar la edicion de la informacion del objeto</t>
+  </si>
+  <si>
+    <t>ENTRADAS: Presionar el boton cancelar</t>
+  </si>
+  <si>
+    <t>EVALUACION: No se realiza ningun cambio en la informacion del objeto.</t>
+  </si>
+  <si>
+    <t>RESULTADO ESPERADO: El objeto publicado mantiene la informacion que tenia antes.</t>
+  </si>
+  <si>
+    <t>1.11</t>
+  </si>
+  <si>
+    <t>1.12</t>
+  </si>
+  <si>
+    <t>1.13</t>
+  </si>
+  <si>
+    <t>Cuando encuentra al menos un objeto en el mercado</t>
+  </si>
+  <si>
+    <t>Cuando no encuentra ningun objeto</t>
+  </si>
+  <si>
+    <t>Buscador vacio</t>
+  </si>
+  <si>
+    <t>Buscar mas de una palabra</t>
+  </si>
+  <si>
+    <t>CONDICIONES DE EJECUCION: Ingresar al mercado de la aplicacion</t>
+  </si>
+  <si>
+    <t>ENTRADAS: Ingresar al mercado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESULTADO ESPERADO: Que se muestre el objeto que esta disponible en el mercado </t>
+  </si>
+  <si>
+    <t>DESCRIPCION: Cuando se ingresa al mercado se mostraran todos los objeto que estan disponible en el mercado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVALUACION: Al ingresa al mercado se ven todos los objetos que han sido publicado por los usuarios junto a su foto. </t>
+  </si>
+  <si>
+    <t>DESCRIPCION: Al ingresar al mercado si este esta vacio debe aparecer un mensaje avisando de que el mercado esta sin objetos</t>
+  </si>
+  <si>
+    <t>CONDICIONES DE EJECUCION: Ingresar al mercado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESULTADO ESPERADO: Se mostrara un mensaje para hacerle saber al usuario que el mercado esta vacio </t>
+  </si>
+  <si>
+    <t>EVALUACION: Efectivamente cuando el mercado esta vacio aparece un mensaje.</t>
+  </si>
+  <si>
+    <t>DESCRIPCION: Si no se a escrito nada en la barra de busqueda en el mercado se deberian mostrar todos los objetos que estan disponibles en el mercado</t>
+  </si>
+  <si>
+    <t>RESULTADO ESPERADO: Se deben mostrar todos los objetos disponibles en el mercado ya que no se ha realizado ninguna busqueda atravez de la barra de busqueda.</t>
+  </si>
+  <si>
+    <t>CONDICIONES DE EJECUCION: Ingresar al mercado y que la barra de busqueda este sin ninugn texto escrito.</t>
+  </si>
+  <si>
+    <t>ENTRADAS: Ingresar al mercado y no haber escrito nada en la barra de busqueda.</t>
+  </si>
+  <si>
+    <t>EVALUACION: Efectivamente al ingresar al mercado y no escribir nada en la barra de busqueda se muestran todos los objetos disponibles en el mercado.</t>
+  </si>
+  <si>
+    <t>DESCRIPCION: Al ingresar al mercado y escribir un objeto en la barra de busqueda los objetos que contengan esa palabra o parecida apareceran en el mercado lo que reducira la cantidad de objetos mostrados por pantalla ya que ahora no se muestran todos los objetos que han sido publicados por los usuarios.</t>
+  </si>
+  <si>
+    <t>CONDICIONES DE EJECUCION: Escribir en la barra de busqueda.</t>
+  </si>
+  <si>
+    <t>ENTRADAS: Ingresar al mercado y escribir una palabra en la barra de busqueda.</t>
+  </si>
+  <si>
+    <t>RESULTADO ESPERADO: Que se pueda encontrar encontrar los objetos buscados en caso de que esten.</t>
+  </si>
+  <si>
+    <t>EVALUACION: Al escribir en la barra de busqueda se muestran objetos relacionados a la palabra ingresada.</t>
+  </si>
+  <si>
+    <t>1.14</t>
+  </si>
+  <si>
+    <t>1.15</t>
+  </si>
+  <si>
+    <t>1.16</t>
+  </si>
+  <si>
+    <t>Categoria con al menos un objeto</t>
+  </si>
+  <si>
+    <t>Categoria sin objetos</t>
+  </si>
+  <si>
+    <t>DESCRIPCION: Al realizar una busqueda filtrada por categoria, se mostrara por pantalla todos los objetos referentes a esa categoria.</t>
+  </si>
+  <si>
+    <t>DESCRIPCION: Si al buscar una busqueda filtrada por categoria de alguna que este sin objetos, no se deberia poder mostrar nada por pantalla salvo un mensaje diciendo que no se encontraron resultados</t>
+  </si>
+  <si>
+    <t>CONDICIONES DE EJECUCION: Entrar al mercado y realizar una busqueda filtrada por categoria.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENTRADAS: Elegir una categoria de las disponibles a la hora de buscar </t>
+  </si>
+  <si>
+    <t>RESULTADO ESPERADO: No se mostrara ningun objeto ya que esa categoria no contiene ninguno asi que solo se deberia mostrar un mensaje de que no se encontraron resultados.</t>
+  </si>
+  <si>
+    <t>RESULTADO ESPERADO: Se mostraran los objetos que pertenecen a esa categoria.</t>
+  </si>
+  <si>
+    <t>EVALUACION: Efectivamente aparece el mensaje de que no se encontraron resultados.</t>
+  </si>
+  <si>
+    <t>EVALUACION: Se muestra por pantalla los objetos pertenecientes a esa categoria.</t>
+  </si>
+  <si>
+    <t>visualizacion de informacion exitosa</t>
+  </si>
+  <si>
+    <t>DESCRIPCION:  Al ingresar al mercado y seleccionar alguno de los objeto se puede visualizar toda la informacion relevante a ese objeto.</t>
+  </si>
+  <si>
+    <t>CONDICIONES DE EJECUCION: Seleccionar uno de los objetos disponibles en el mercado.</t>
+  </si>
+  <si>
+    <t>ENTRADAS: Seleccionar un objeto del mercado</t>
+  </si>
+  <si>
+    <t>RESULTADO ESPERADO: Se muestra en la pantalla toda la informacion de la pulbicacion de ese objeto.</t>
+  </si>
+  <si>
+    <t>EVALUACION: Efectivamente al presionar alguno de los objetos se muestra por pantalla la informacion de este.</t>
   </si>
 </sst>
 </file>
@@ -3018,8 +3211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B871C4F-8534-4669-84CE-6EC951CCDC87}">
   <dimension ref="B2:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11:R16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17:R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3098,7 +3291,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -3110,7 +3303,7 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
@@ -3119,7 +3312,7 @@
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -3129,7 +3322,7 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="K7" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
@@ -3195,7 +3388,7 @@
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -3204,16 +3397,16 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="K11" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
+      <c r="K11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
@@ -3224,14 +3417,14 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
@@ -3242,14 +3435,14 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
@@ -3260,14 +3453,14 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
@@ -3278,14 +3471,14 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
@@ -3296,18 +3489,18 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -3317,7 +3510,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="K17" s="3" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
@@ -3383,7 +3576,7 @@
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -3392,16 +3585,16 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
-      <c r="K21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
+      <c r="K21" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
@@ -3412,14 +3605,14 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
@@ -3430,18 +3623,18 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -3450,16 +3643,16 @@
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
-      <c r="K24" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
+      <c r="K24" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
@@ -3470,14 +3663,14 @@
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
@@ -3488,14 +3681,14 @@
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="3"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
@@ -3506,14 +3699,14 @@
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="3"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -3540,4 +3733,2390 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{154E1C07-258C-477D-BAC9-C0346789DE1C}">
+  <dimension ref="B2:R27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V25" sqref="V25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="2">
+        <v>3</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="K6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="K7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="K11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="K17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="K21" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="K24" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="B24:I27"/>
+    <mergeCell ref="K24:R27"/>
+    <mergeCell ref="B17:I20"/>
+    <mergeCell ref="K17:R20"/>
+    <mergeCell ref="B21:I23"/>
+    <mergeCell ref="K21:R23"/>
+    <mergeCell ref="B7:I10"/>
+    <mergeCell ref="K7:R10"/>
+    <mergeCell ref="B11:I16"/>
+    <mergeCell ref="K11:R16"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:I6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="O5:Q5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C56C667B-8265-47E3-B6C6-0883A60D21F2}">
+  <dimension ref="B2:AA52"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11:AA16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="T4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
+    </row>
+    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="2">
+        <v>5</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="2">
+        <v>5</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="K6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="T6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="4"/>
+    </row>
+    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="K7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="T7" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="5"/>
+    </row>
+    <row r="8" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="5"/>
+    </row>
+    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="5"/>
+    </row>
+    <row r="10" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="5"/>
+    </row>
+    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="K11" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="T11" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="5"/>
+    </row>
+    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="5"/>
+    </row>
+    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="5"/>
+    </row>
+    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="5"/>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="5"/>
+      <c r="Z15" s="5"/>
+      <c r="AA15" s="5"/>
+    </row>
+    <row r="16" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="5"/>
+      <c r="Z16" s="5"/>
+      <c r="AA16" s="5"/>
+    </row>
+    <row r="17" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="K17" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="T17" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AA17" s="3"/>
+    </row>
+    <row r="18" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3"/>
+      <c r="V18" s="3"/>
+      <c r="W18" s="3"/>
+      <c r="X18" s="3"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3"/>
+      <c r="AA18" s="3"/>
+    </row>
+    <row r="19" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
+      <c r="AA19" s="3"/>
+    </row>
+    <row r="20" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3"/>
+      <c r="AA20" s="3"/>
+    </row>
+    <row r="21" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="K21" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="T21" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5"/>
+      <c r="W21" s="5"/>
+      <c r="X21" s="5"/>
+      <c r="Y21" s="5"/>
+      <c r="Z21" s="5"/>
+      <c r="AA21" s="5"/>
+    </row>
+    <row r="22" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
+      <c r="V22" s="5"/>
+      <c r="W22" s="5"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="5"/>
+    </row>
+    <row r="23" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="T23" s="5"/>
+      <c r="U23" s="5"/>
+      <c r="V23" s="5"/>
+      <c r="W23" s="5"/>
+      <c r="X23" s="5"/>
+      <c r="Y23" s="5"/>
+      <c r="Z23" s="5"/>
+      <c r="AA23" s="5"/>
+    </row>
+    <row r="24" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="K24" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="T24" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="U24" s="5"/>
+      <c r="V24" s="5"/>
+      <c r="W24" s="5"/>
+      <c r="X24" s="5"/>
+      <c r="Y24" s="5"/>
+      <c r="Z24" s="5"/>
+      <c r="AA24" s="5"/>
+    </row>
+    <row r="25" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="T25" s="5"/>
+      <c r="U25" s="5"/>
+      <c r="V25" s="5"/>
+      <c r="W25" s="5"/>
+      <c r="X25" s="5"/>
+      <c r="Y25" s="5"/>
+      <c r="Z25" s="5"/>
+      <c r="AA25" s="5"/>
+    </row>
+    <row r="26" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5"/>
+      <c r="W26" s="5"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="5"/>
+      <c r="AA26" s="5"/>
+    </row>
+    <row r="27" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
+      <c r="X27" s="5"/>
+      <c r="Y27" s="5"/>
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="5"/>
+    </row>
+    <row r="29" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+    </row>
+    <row r="32" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="40">
+    <mergeCell ref="B49:I52"/>
+    <mergeCell ref="B36:I41"/>
+    <mergeCell ref="B42:I45"/>
+    <mergeCell ref="B46:I48"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="E31:I31"/>
+    <mergeCell ref="B32:I35"/>
+    <mergeCell ref="B24:I27"/>
+    <mergeCell ref="K24:R27"/>
+    <mergeCell ref="T24:AA27"/>
+    <mergeCell ref="B29:I29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B17:I20"/>
+    <mergeCell ref="K17:R20"/>
+    <mergeCell ref="T17:AA20"/>
+    <mergeCell ref="B21:I23"/>
+    <mergeCell ref="K21:R23"/>
+    <mergeCell ref="T21:AA23"/>
+    <mergeCell ref="B7:I10"/>
+    <mergeCell ref="K7:R10"/>
+    <mergeCell ref="T7:AA10"/>
+    <mergeCell ref="B11:I16"/>
+    <mergeCell ref="K11:R16"/>
+    <mergeCell ref="T11:AA16"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:I6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="T6:V6"/>
+    <mergeCell ref="W6:AA6"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="T4:AA4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="T5:V5"/>
+    <mergeCell ref="X5:Z5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04B415D-EF40-48DE-9CF5-25E90BFE3A39}">
+  <dimension ref="B2:R27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K24" sqref="K24:R27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="2">
+        <v>8</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="K6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="K7" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="K11" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="K17" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="K21" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="K24" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="B24:I27"/>
+    <mergeCell ref="K24:R27"/>
+    <mergeCell ref="B17:I20"/>
+    <mergeCell ref="K17:R20"/>
+    <mergeCell ref="B21:I23"/>
+    <mergeCell ref="K21:R23"/>
+    <mergeCell ref="B7:I10"/>
+    <mergeCell ref="K7:R10"/>
+    <mergeCell ref="B11:I16"/>
+    <mergeCell ref="K11:R16"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:I6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="O5:Q5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55EB57AB-2015-49BA-ACD1-880EC1F5B642}">
+  <dimension ref="B2:J27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:I27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B24:I27"/>
+    <mergeCell ref="B17:I20"/>
+    <mergeCell ref="B21:I23"/>
+    <mergeCell ref="B7:I10"/>
+    <mergeCell ref="B11:I16"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:I6"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="F5:H5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>